<commit_message>
Final code for BalticSea project
</commit_message>
<xml_diff>
--- a/Transect_16S_data/Training Data/easy_get_para.xlsx
+++ b/Transect_16S_data/Training Data/easy_get_para.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="15880" yWindow="1160" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
   <si>
     <t>Depth</t>
   </si>
@@ -630,6 +630,9 @@
   </si>
   <si>
     <t>W190</t>
+  </si>
+  <si>
+    <t>salinity</t>
   </si>
 </sst>
 </file>
@@ -725,8 +728,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -747,11 +754,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1027,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,7 +1051,7 @@
     <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1054,8 +1065,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1071,8 +1085,11 @@
       <c r="E2">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>10.5063</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1088,8 +1105,11 @@
       <c r="E3">
         <v>17.736499999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>6.5331000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1105,8 +1125,11 @@
       <c r="E4">
         <v>17.3535</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>7.4904999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1122,8 +1145,11 @@
       <c r="E5">
         <v>17.3535</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>5.9172000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1139,8 +1165,11 @@
       <c r="E6">
         <v>17.3535</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>7.1520999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1156,8 +1185,11 @@
       <c r="E7">
         <v>17.353833330000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>5.6105999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -1173,8 +1205,11 @@
       <c r="E8">
         <v>17.353833330000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>6.0345000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1190,8 +1225,11 @@
       <c r="E9">
         <v>17.353833330000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>7.6611000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1207,8 +1245,11 @@
       <c r="E10">
         <v>16.950833329999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>6.5148999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1224,8 +1265,11 @@
       <c r="E11">
         <v>16.950833329999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>5.0468999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1241,8 +1285,11 @@
       <c r="E12">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>7.6878000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -1258,8 +1305,11 @@
       <c r="E13">
         <v>16.950833329999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>7.7207999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1275,8 +1325,11 @@
       <c r="E14">
         <v>16.513000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>7.3827999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
@@ -1292,8 +1345,11 @@
       <c r="E15">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>8.0155999999999992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
@@ -1309,8 +1365,11 @@
       <c r="E16">
         <v>22.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>7.5087999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
@@ -1326,8 +1385,11 @@
       <c r="E17">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>12.0845</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1343,8 +1405,11 @@
       <c r="E18">
         <v>19.466388999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>5.6573000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -1360,8 +1425,11 @@
       <c r="E19">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>7.6372999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
@@ -1377,8 +1445,11 @@
       <c r="E20">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -1394,8 +1465,11 @@
       <c r="E21">
         <v>17.353899999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>7.5820000000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -1411,8 +1485,11 @@
       <c r="E22">
         <v>16.52167</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>8.6876999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -1428,8 +1505,11 @@
       <c r="E23">
         <v>13.30111</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>12.0641</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
@@ -1445,8 +1525,11 @@
       <c r="E24">
         <v>10.887499999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>13.3055</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
@@ -1462,8 +1545,11 @@
       <c r="E25">
         <v>10.887499999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>13.911099999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
@@ -1479,8 +1565,11 @@
       <c r="E26">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>7.5128000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
@@ -1496,8 +1585,11 @@
       <c r="E27">
         <v>11.05</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>27.226700000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>30</v>
       </c>
@@ -1513,8 +1605,11 @@
       <c r="E28">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>29.850999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
@@ -1530,8 +1625,11 @@
       <c r="E29">
         <v>10.82</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>30.588699999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
@@ -1547,8 +1645,11 @@
       <c r="E30">
         <v>11.11</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>30.817799999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
@@ -1564,8 +1665,11 @@
       <c r="E31">
         <v>12.27</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>17.377700000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>34</v>
       </c>
@@ -1581,8 +1685,11 @@
       <c r="E32">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>16.953900000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
@@ -1598,8 +1705,11 @@
       <c r="E33">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>7.6786000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>36</v>
       </c>
@@ -1615,8 +1725,11 @@
       <c r="E34">
         <v>12.27</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>23.2834</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
@@ -1632,8 +1745,11 @@
       <c r="E35">
         <v>12.27</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>28.573799999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>38</v>
       </c>
@@ -1649,8 +1765,11 @@
       <c r="E36">
         <v>11.08</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>20.4023</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
@@ -1666,8 +1785,11 @@
       <c r="E37">
         <v>11.08</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>26.640899999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>40</v>
       </c>
@@ -1683,8 +1805,11 @@
       <c r="E38">
         <v>11.94</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>19.168600000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
@@ -1700,8 +1825,11 @@
       <c r="E39">
         <v>11.94</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>30.0855</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>42</v>
       </c>
@@ -1717,8 +1845,11 @@
       <c r="E40">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>11.167999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>43</v>
       </c>
@@ -1734,8 +1865,11 @@
       <c r="E41">
         <v>11.94</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>33.767000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>44</v>
       </c>
@@ -1751,8 +1885,11 @@
       <c r="E42">
         <v>11.17</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>23.779199999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>45</v>
       </c>
@@ -1768,8 +1905,11 @@
       <c r="E43">
         <v>11.17</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>30.901800000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>46</v>
       </c>
@@ -1785,8 +1925,11 @@
       <c r="E44">
         <v>11.17</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>33.0197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>47</v>
       </c>
@@ -1802,8 +1945,11 @@
       <c r="E45">
         <v>11.17</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>34.057699999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>48</v>
       </c>
@@ -1819,8 +1965,11 @@
       <c r="E46">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>26.9297</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>49</v>
       </c>
@@ -1836,8 +1985,11 @@
       <c r="E47">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>30.998200000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>50</v>
       </c>
@@ -1853,8 +2005,11 @@
       <c r="E48">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>32.511200000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>51</v>
       </c>
@@ -1870,8 +2025,11 @@
       <c r="E49">
         <v>10.28</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>30.6325</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>52</v>
       </c>
@@ -1887,8 +2045,11 @@
       <c r="E50">
         <v>10.28</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>33.512099999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>53</v>
       </c>
@@ -1904,8 +2065,11 @@
       <c r="E51">
         <v>10.28</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>35.165599999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>54</v>
       </c>
@@ -1921,8 +2085,11 @@
       <c r="E52">
         <v>10.28</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>35.165599999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>55</v>
       </c>
@@ -1938,8 +2105,11 @@
       <c r="E53">
         <v>10.28</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>35.209499999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
@@ -1955,8 +2125,11 @@
       <c r="E54">
         <v>10.3</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>30.9177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>57</v>
       </c>
@@ -1972,8 +2145,11 @@
       <c r="E55">
         <v>10.3</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>33.827399999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>58</v>
       </c>
@@ -1989,8 +2165,11 @@
       <c r="E56">
         <v>17.8</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>7.4910000000000014</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>59</v>
       </c>
@@ -2006,8 +2185,11 @@
       <c r="E57">
         <v>17.8</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>8.2661999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>60</v>
       </c>
@@ -2023,8 +2205,11 @@
       <c r="E58">
         <v>17.8</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>11.268800000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>61</v>
       </c>
@@ -2040,8 +2225,11 @@
       <c r="E59">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>7.2260999999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>62</v>
       </c>
@@ -2057,8 +2245,11 @@
       <c r="E60">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>7.4745999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>63</v>
       </c>
@@ -2074,8 +2265,11 @@
       <c r="E61">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>8.3788</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>64</v>
       </c>
@@ -2091,8 +2285,11 @@
       <c r="E62">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>7.7389999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>65</v>
       </c>
@@ -2108,8 +2305,11 @@
       <c r="E63">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>7.3756000000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>66</v>
       </c>
@@ -2125,8 +2325,11 @@
       <c r="E64">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>7.3935000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>67</v>
       </c>
@@ -2142,8 +2345,11 @@
       <c r="E65">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>7.4015000000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
@@ -2159,8 +2365,11 @@
       <c r="E66">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>8.6372999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>69</v>
       </c>
@@ -2176,8 +2385,11 @@
       <c r="E67">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>11.479900000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>70</v>
       </c>
@@ -2193,8 +2405,11 @@
       <c r="E68">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>7.2546999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>71</v>
       </c>
@@ -2210,8 +2425,11 @@
       <c r="E69">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>8.8210999999999995</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>72</v>
       </c>
@@ -2227,8 +2445,11 @@
       <c r="E70">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>7.1170000000000009</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>73</v>
       </c>
@@ -2244,8 +2465,11 @@
       <c r="E71">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>7.4086999999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>74</v>
       </c>
@@ -2261,8 +2485,11 @@
       <c r="E72">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>8.0538000000000007</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>75</v>
       </c>
@@ -2278,8 +2505,11 @@
       <c r="E73">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <v>6.2450000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>76</v>
       </c>
@@ -2295,8 +2525,11 @@
       <c r="E74">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>77</v>
       </c>
@@ -2312,8 +2545,11 @@
       <c r="E75">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>78</v>
       </c>
@@ -2329,8 +2565,11 @@
       <c r="E76">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>79</v>
       </c>
@@ -2346,8 +2585,11 @@
       <c r="E77">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>5.3132999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>80</v>
       </c>
@@ -2363,8 +2605,11 @@
       <c r="E78">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>2.5741000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>81</v>
       </c>
@@ -2380,8 +2625,11 @@
       <c r="E79">
         <v>22.1</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <v>2.8483999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>82</v>
       </c>
@@ -2397,8 +2645,11 @@
       <c r="E80">
         <v>16</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>7.5385</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>83</v>
       </c>
@@ -2414,8 +2665,11 @@
       <c r="E81">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>4.9470000000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>84</v>
       </c>
@@ -2431,8 +2685,11 @@
       <c r="E82">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>5.0907999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>85</v>
       </c>
@@ -2448,8 +2705,11 @@
       <c r="E83">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>5.4378000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>86</v>
       </c>
@@ -2465,8 +2725,11 @@
       <c r="E84">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>6.0868000000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>87</v>
       </c>
@@ -2482,8 +2745,11 @@
       <c r="E85">
         <v>20</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>4.7709000000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>88</v>
       </c>
@@ -2499,8 +2765,11 @@
       <c r="E86">
         <v>10.8788567</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>23.969200000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>89</v>
       </c>
@@ -2516,8 +2785,11 @@
       <c r="E87">
         <v>11.0553983</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>29.220800000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>90</v>
       </c>
@@ -2533,8 +2805,11 @@
       <c r="E88">
         <v>10.8089917</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>15.842599999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>91</v>
       </c>
@@ -2550,8 +2825,11 @@
       <c r="E89">
         <v>10.8089917</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>30.9544</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>92</v>
       </c>
@@ -2567,8 +2845,11 @@
       <c r="E90">
         <v>11.109831700000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>18.674700000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>93</v>
       </c>
@@ -2584,8 +2865,11 @@
       <c r="E91">
         <v>11.109831700000001</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>32.374499999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>94</v>
       </c>
@@ -2601,8 +2885,11 @@
       <c r="E92">
         <v>11.071960000000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>29.520700000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>95</v>
       </c>
@@ -2618,8 +2905,11 @@
       <c r="E93">
         <v>11.664</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>34.277200000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>96</v>
       </c>
@@ -2635,8 +2925,11 @@
       <c r="E94">
         <v>11.664</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>34.7483</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>97</v>
       </c>
@@ -2652,8 +2945,11 @@
       <c r="E95">
         <v>11.093075000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>20.214400000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>98</v>
       </c>
@@ -2669,8 +2965,11 @@
       <c r="E96">
         <v>11.093075000000001</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>32.240600000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>99</v>
       </c>
@@ -2686,8 +2985,11 @@
       <c r="E97">
         <v>11.093075000000001</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>34.1051</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>100</v>
       </c>
@@ -2703,8 +3005,11 @@
       <c r="E98">
         <v>10.2740917</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>34.104100000000003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>101</v>
       </c>
@@ -2720,8 +3025,11 @@
       <c r="E99">
         <v>10.2740917</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>35.005400000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>102</v>
       </c>
@@ -2737,8 +3045,11 @@
       <c r="E100">
         <v>10.2740917</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>34.974400000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>103</v>
       </c>
@@ -2754,8 +3065,11 @@
       <c r="E101">
         <v>10.2960917</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>26.972999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>104</v>
       </c>
@@ -2771,8 +3085,11 @@
       <c r="E102">
         <v>10.2960917</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>34.6663</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>105</v>
       </c>
@@ -2788,8 +3105,11 @@
       <c r="E103">
         <v>10.2960917</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103">
+        <v>35.006399999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>106</v>
       </c>
@@ -2805,8 +3125,11 @@
       <c r="E104">
         <v>10.2960917</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <v>35.2089</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>107</v>
       </c>
@@ -2822,8 +3145,11 @@
       <c r="E105">
         <v>11.9330917</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <v>19.4498</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>108</v>
       </c>
@@ -2839,8 +3165,11 @@
       <c r="E106">
         <v>11.9330917</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <v>33.421300000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>109</v>
       </c>
@@ -2856,8 +3185,11 @@
       <c r="E107">
         <v>11.9330917</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <v>34.353099999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>110</v>
       </c>
@@ -2873,8 +3205,11 @@
       <c r="E108">
         <v>12.2652617</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <v>31.770299999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>111</v>
       </c>
@@ -2890,8 +3225,11 @@
       <c r="E109">
         <v>13.3008817</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <v>8.3865999999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>112</v>
       </c>
@@ -2907,8 +3245,11 @@
       <c r="E110">
         <v>14.438001699999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110">
+        <v>8.3872999999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>113</v>
       </c>
@@ -2924,8 +3265,11 @@
       <c r="E111">
         <v>14.438001699999999</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111">
+        <v>14.138999999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>114</v>
       </c>
@@ -2941,8 +3285,11 @@
       <c r="E112">
         <v>14.91986</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112">
+        <v>7.7417999999999996</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>115</v>
       </c>
@@ -2958,8 +3305,11 @@
       <c r="E113">
         <v>14.91986</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113">
+        <v>7.7472000000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>116</v>
       </c>
@@ -2975,8 +3325,11 @@
       <c r="E114">
         <v>14.91986</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114">
+        <v>7.8606999999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>117</v>
       </c>
@@ -2992,8 +3345,11 @@
       <c r="E115">
         <v>15.5695383</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115">
+        <v>7.7625999999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>118</v>
       </c>
@@ -3009,8 +3365,11 @@
       <c r="E116">
         <v>15.5695383</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116">
+        <v>7.8478000000000003</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>119</v>
       </c>
@@ -3026,8 +3385,11 @@
       <c r="E117">
         <v>16.514083299999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117">
+        <v>7.3813000000000004</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>120</v>
       </c>
@@ -3043,8 +3405,11 @@
       <c r="E118">
         <v>16.514083299999999</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118">
+        <v>7.4089999999999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>121</v>
       </c>
@@ -3060,8 +3425,11 @@
       <c r="E119">
         <v>16.514083299999999</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119">
+        <v>7.1706000000000003</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>122</v>
       </c>
@@ -3077,8 +3445,11 @@
       <c r="E120">
         <v>16.950385000000001</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120">
+        <v>7.1788999999999996</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>123</v>
       </c>
@@ -3094,8 +3465,11 @@
       <c r="E121">
         <v>16.950385000000001</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121">
+        <v>7.1952999999999996</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>124</v>
       </c>
@@ -3111,8 +3485,11 @@
       <c r="E122">
         <v>17.354001700000001</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F122">
+        <v>7.1417999999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>125</v>
       </c>
@@ -3128,8 +3505,11 @@
       <c r="E123">
         <v>17.354001700000001</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123">
+        <v>7.1943000000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>126</v>
       </c>
@@ -3145,8 +3525,11 @@
       <c r="E124">
         <v>17.580778299999999</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124">
+        <v>7.0949</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>127</v>
       </c>
@@ -3162,8 +3545,11 @@
       <c r="E125">
         <v>17.580778299999999</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125">
+        <v>7.1471999999999998</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>128</v>
       </c>
@@ -3179,8 +3565,11 @@
       <c r="E126">
         <v>17.580778299999999</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F126">
+        <v>8.4415999999999993</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>129</v>
       </c>
@@ -3196,8 +3585,11 @@
       <c r="E127">
         <v>17.352399999999999</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F127">
+        <v>7.0068000000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>130</v>
       </c>
@@ -3213,8 +3605,11 @@
       <c r="E128">
         <v>17.352399999999999</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F128">
+        <v>7.0746000000000002</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>131</v>
       </c>
@@ -3230,8 +3625,11 @@
       <c r="E129">
         <v>17.736678300000001</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129">
+        <v>6.9053000000000004</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>132</v>
       </c>
@@ -3247,8 +3645,11 @@
       <c r="E130">
         <v>17.736678300000001</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F130">
+        <v>7.0063000000000004</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>133</v>
       </c>
@@ -3264,8 +3665,11 @@
       <c r="E131">
         <v>18.2334733</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131">
+        <v>6.4503000000000004</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>134</v>
       </c>
@@ -3281,8 +3685,11 @@
       <c r="E132">
         <v>18.2334733</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F132">
+        <v>6.9866999999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>135</v>
       </c>
@@ -3298,8 +3705,11 @@
       <c r="E133">
         <v>18.2334733</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133">
+        <v>7.0636000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>136</v>
       </c>
@@ -3315,8 +3725,11 @@
       <c r="E134">
         <v>19.0960067</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134">
+        <v>7.0286</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>137</v>
       </c>
@@ -3332,8 +3745,11 @@
       <c r="E135">
         <v>19.459129999999998</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F135">
+        <v>6.4413</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>138</v>
       </c>
@@ -3349,8 +3765,11 @@
       <c r="E136">
         <v>19.459129999999998</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F136">
+        <v>6.8430999999999997</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>139</v>
       </c>
@@ -3366,8 +3785,11 @@
       <c r="E137">
         <v>19.459129999999998</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F137">
+        <v>7.6166999999999998</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>140</v>
       </c>
@@ -3383,8 +3805,11 @@
       <c r="E138">
         <v>19.11769</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F138">
+        <v>5.4230999999999998</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>141</v>
       </c>
@@ -3400,8 +3825,11 @@
       <c r="E139">
         <v>19.11769</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F139">
+        <v>6.4390000000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>142</v>
       </c>
@@ -3417,8 +3845,11 @@
       <c r="E140">
         <v>19.11769</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140">
+        <v>6.6433</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>143</v>
       </c>
@@ -3434,8 +3865,11 @@
       <c r="E141">
         <v>19.11769</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F141">
+        <v>7.0525000000000002</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>144</v>
       </c>
@@ -3451,8 +3885,11 @@
       <c r="E142">
         <v>19.7181517</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F142">
+        <v>5.4489999999999998</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>145</v>
       </c>
@@ -3468,8 +3905,11 @@
       <c r="E143">
         <v>19.7181517</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F143">
+        <v>6.2736000000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>146</v>
       </c>
@@ -3485,8 +3925,11 @@
       <c r="E144">
         <v>19.9681967</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F144">
+        <v>5.5183</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>147</v>
       </c>
@@ -3502,8 +3945,11 @@
       <c r="E145">
         <v>19.9681967</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F145">
+        <v>5.5454999999999997</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>148</v>
       </c>
@@ -3519,8 +3965,11 @@
       <c r="E146">
         <v>19.9681967</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F146">
+        <v>5.7164000000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>149</v>
       </c>
@@ -3536,8 +3985,11 @@
       <c r="E147">
         <v>19.9681967</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F147">
+        <v>6.3160999999999996</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>150</v>
       </c>
@@ -3553,8 +4005,11 @@
       <c r="E148">
         <v>20.486201699999999</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F148">
+        <v>5.5399000000000003</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>151</v>
       </c>
@@ -3570,8 +4025,11 @@
       <c r="E149">
         <v>20.486201699999999</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F149">
+        <v>5.5486000000000004</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>152</v>
       </c>
@@ -3587,8 +4045,11 @@
       <c r="E150">
         <v>20.486201699999999</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F150">
+        <v>5.5521000000000003</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>153</v>
       </c>
@@ -3604,8 +4065,11 @@
       <c r="E151">
         <v>20.486201699999999</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F151">
+        <v>5.5709</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>154</v>
       </c>
@@ -3621,8 +4085,11 @@
       <c r="E152">
         <v>25.63252</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F152">
+        <v>5.0864000000000003</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>155</v>
       </c>
@@ -3638,8 +4105,11 @@
       <c r="E153">
         <v>25.63252</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F153">
+        <v>9.0937000000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>156</v>
       </c>
@@ -3655,8 +4125,11 @@
       <c r="E154">
         <v>24.8498333</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F154">
+        <v>5.2415000000000003</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>157</v>
       </c>
@@ -3672,8 +4145,11 @@
       <c r="E155">
         <v>24.8498333</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F155">
+        <v>5.3045</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>158</v>
       </c>
@@ -3689,8 +4165,11 @@
       <c r="E156">
         <v>24.8498333</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F156">
+        <v>6.2415000000000003</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>159</v>
       </c>
@@ -3706,8 +4185,11 @@
       <c r="E157">
         <v>24.8498333</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F157">
+        <v>6.9283999999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>160</v>
       </c>
@@ -3723,8 +4205,11 @@
       <c r="E158">
         <v>24.8498333</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F158">
+        <v>9.2897999999999996</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>161</v>
       </c>
@@ -3740,8 +4225,11 @@
       <c r="E159">
         <v>23.998944999999999</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F159">
+        <v>5.8567999999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>162</v>
       </c>
@@ -3757,8 +4245,11 @@
       <c r="E160">
         <v>23.998944999999999</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F160">
+        <v>7.1996000000000002</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>163</v>
       </c>
@@ -3774,8 +4265,11 @@
       <c r="E161">
         <v>23.998944999999999</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F161">
+        <v>6.4231999999999996</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>164</v>
       </c>
@@ -3791,8 +4285,11 @@
       <c r="E162">
         <v>23.998944999999999</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F162">
+        <v>9.1981000000000002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>165</v>
       </c>
@@ -3808,8 +4305,11 @@
       <c r="E163">
         <v>21.000591700000001</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F163">
+        <v>6.3365</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>166</v>
       </c>
@@ -3825,8 +4325,11 @@
       <c r="E164">
         <v>21.000591700000001</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F164">
+        <v>6.4352999999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>167</v>
       </c>
@@ -3842,8 +4345,11 @@
       <c r="E165">
         <v>21.000591700000001</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F165">
+        <v>6.5644999999999998</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>168</v>
       </c>
@@ -3859,8 +4365,11 @@
       <c r="E166">
         <v>21.000591700000001</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F166">
+        <v>6.7465999999999999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>169</v>
       </c>
@@ -3876,8 +4385,11 @@
       <c r="E167">
         <v>21.368393300000001</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F167">
+        <v>6.9965000000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>170</v>
       </c>
@@ -3893,8 +4405,11 @@
       <c r="E168">
         <v>21.368393300000001</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F168">
+        <v>7.0420000000000007</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>171</v>
       </c>
@@ -3910,8 +4425,11 @@
       <c r="E169">
         <v>20.350349999999999</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F169">
+        <v>7.4972000000000003</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>172</v>
       </c>
@@ -3927,8 +4445,11 @@
       <c r="E170">
         <v>20.09</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F170">
+        <v>7.2293000000000003</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>173</v>
       </c>
@@ -3944,8 +4465,11 @@
       <c r="E171">
         <v>20.09</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F171">
+        <v>7.2641</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>174</v>
       </c>
@@ -3961,8 +4485,11 @@
       <c r="E172">
         <v>20.0745</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F172">
+        <v>7.3270000000000008</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>175</v>
       </c>
@@ -3978,8 +4505,11 @@
       <c r="E173">
         <v>20.0745</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F173">
+        <v>7.3289999999999997</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>176</v>
       </c>
@@ -3995,8 +4525,11 @@
       <c r="E174">
         <v>20.0745</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F174">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>177</v>
       </c>
@@ -4012,8 +4545,11 @@
       <c r="E175">
         <v>19.7083333</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F175">
+        <v>7.3958000000000004</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>178</v>
       </c>
@@ -4029,8 +4565,11 @@
       <c r="E176">
         <v>19.7083333</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F176">
+        <v>7.5639000000000003</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>179</v>
       </c>
@@ -4046,8 +4585,11 @@
       <c r="E177">
         <v>18.991</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F177">
+        <v>7.5399000000000003</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>180</v>
       </c>
@@ -4063,8 +4605,11 @@
       <c r="E178">
         <v>18.991</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F178">
+        <v>7.6201999999999996</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>181</v>
       </c>
@@ -4080,8 +4625,11 @@
       <c r="E179">
         <v>18.991</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F179">
+        <v>11.8423</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>182</v>
       </c>
@@ -4097,8 +4645,11 @@
       <c r="E180">
         <v>18.400833299999999</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F180">
+        <v>7.4489999999999998</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>183</v>
       </c>
@@ -4114,8 +4665,11 @@
       <c r="E181">
         <v>18.400833299999999</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F181">
+        <v>7.4687999999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>184</v>
       </c>
@@ -4131,8 +4685,11 @@
       <c r="E182">
         <v>19.283983299999999</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F182">
+        <v>7.5086000000000004</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>185</v>
       </c>
@@ -4148,8 +4705,11 @@
       <c r="E183">
         <v>19.283983299999999</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F183">
+        <v>7.7554999999999996</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>186</v>
       </c>
@@ -4165,8 +4725,11 @@
       <c r="E184">
         <v>17.80705</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F184">
+        <v>7.6214000000000004</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>187</v>
       </c>
@@ -4182,8 +4745,11 @@
       <c r="E185">
         <v>17.80705</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F185">
+        <v>12.2316</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>188</v>
       </c>
@@ -4199,8 +4765,11 @@
       <c r="E186">
         <v>17.80705</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F186">
+        <v>13.254799999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>189</v>
       </c>
@@ -4216,8 +4785,11 @@
       <c r="E187">
         <v>15.9839333</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F187">
+        <v>7.8562000000000003</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>190</v>
       </c>
@@ -4233,8 +4805,11 @@
       <c r="E188">
         <v>15.382383300000001</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F188">
+        <v>7.7967000000000004</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>191</v>
       </c>
@@ -4250,8 +4825,11 @@
       <c r="E189">
         <v>15.382383300000001</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F189">
+        <v>12.527900000000001</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>192</v>
       </c>
@@ -4267,8 +4845,11 @@
       <c r="E190">
         <v>15.382383300000001</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F190">
+        <v>13.638299999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>193</v>
       </c>
@@ -4284,8 +4865,11 @@
       <c r="E191">
         <v>13.499650000000001</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F191">
+        <v>8.1902000000000008</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>194</v>
       </c>
@@ -4301,8 +4885,11 @@
       <c r="E192">
         <v>13.499650000000001</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F192">
+        <v>12.813000000000001</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
         <v>195</v>
       </c>
@@ -4318,8 +4905,11 @@
       <c r="E193">
         <v>13.499650000000001</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F193">
+        <v>15.6258</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>196</v>
       </c>
@@ -4335,8 +4925,11 @@
       <c r="E194">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F194">
+        <v>8.8386999999999993</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
         <v>197</v>
       </c>
@@ -4352,8 +4945,11 @@
       <c r="E195">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F195">
+        <v>12.692600000000001</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>198</v>
       </c>
@@ -4369,8 +4965,11 @@
       <c r="E196">
         <v>12.7073833</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F196">
+        <v>8.4507999999999992</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
         <v>199</v>
       </c>
@@ -4386,8 +4985,11 @@
       <c r="E197">
         <v>12.7073833</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F197">
+        <v>12.174200000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
         <v>200</v>
       </c>
@@ -4403,8 +5005,11 @@
       <c r="E198">
         <v>12.103483300000001</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F198">
+        <v>10.1182</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
         <v>201</v>
       </c>
@@ -4419,6 +5024,9 @@
       </c>
       <c r="E199">
         <v>12.103483300000001</v>
+      </c>
+      <c r="F199">
+        <v>16.1812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>